<commit_message>
Able to adjust unit
</commit_message>
<xml_diff>
--- a/backend/data/odds/2021/Week_12.xlsx
+++ b/backend/data/odds/2021/Week_12.xlsx
@@ -512,12 +512,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-350</t>
+          <t>-335</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>+270</t>
+          <t>+260</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -543,12 +543,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+205</t>
+          <t>+190</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-255</t>
+          <t>-235</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -574,12 +574,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-200</t>
+          <t>-210</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>+170</t>
+          <t>+175</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -605,12 +605,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+140</t>
+          <t>+135</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-160</t>
+          <t>-155</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -667,12 +667,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-260</t>
+          <t>-265</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>+210</t>
+          <t>+215</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -698,12 +698,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>+150</t>
+          <t>+155</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-170</t>
+          <t>-180</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -760,12 +760,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>-140</t>
+          <t>-145</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>+120</t>
+          <t>+125</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -791,12 +791,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>+130</t>
+          <t>+125</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-150</t>
+          <t>-145</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -822,12 +822,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>-110</t>
+          <t>-105</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-110</t>
+          <t>-115</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -884,12 +884,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>-180</t>
+          <t>-190</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>+155</t>
+          <t>+160</t>
         </is>
       </c>
       <c r="F15" t="n">

</xml_diff>